<commit_message>
Correção metricas de CK & LK
</commit_message>
<xml_diff>
--- a/docs/metricas de complexidade.xlsx
+++ b/docs/metricas de complexidade.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7905"/>
   </bookViews>
   <sheets>
     <sheet name="Metricas CK &amp; LK" sheetId="1" r:id="rId1"/>
@@ -815,8 +815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +855,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3">
         <v>0</v>
@@ -867,7 +867,7 @@
         <v>3</v>
       </c>
       <c r="F3" s="3">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3">
         <v>0</v>
@@ -881,7 +881,7 @@
         <v>9</v>
       </c>
       <c r="B4" s="3">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="3">
         <v>0</v>
@@ -893,7 +893,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="3">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G4" s="3">
         <v>0</v>
@@ -907,7 +907,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" s="1">
         <v>0</v>
@@ -919,7 +919,7 @@
         <v>2</v>
       </c>
       <c r="F5" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G5" s="1">
         <v>0</v>
@@ -933,7 +933,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C6" s="1">
         <v>0</v>
@@ -945,7 +945,7 @@
         <v>2</v>
       </c>
       <c r="F6" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G6" s="1">
         <v>0</v>
@@ -959,7 +959,7 @@
         <v>12</v>
       </c>
       <c r="B7" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
         <v>0</v>
@@ -971,7 +971,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="1">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G7" s="1">
         <v>0</v>
@@ -985,7 +985,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="3">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C8" s="3">
         <v>0</v>
@@ -997,7 +997,7 @@
         <v>2</v>
       </c>
       <c r="F8" s="3">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G8" s="3">
         <v>0</v>
@@ -1011,7 +1011,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
         <v>0</v>
@@ -1023,7 +1023,7 @@
         <v>0</v>
       </c>
       <c r="F9" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G9" s="1">
         <v>0</v>
@@ -1037,7 +1037,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="1">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C10" s="1">
         <v>0</v>
@@ -1049,7 +1049,7 @@
         <v>0</v>
       </c>
       <c r="F10" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G10" s="1">
         <v>0</v>
@@ -1063,7 +1063,7 @@
         <v>16</v>
       </c>
       <c r="B11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1">
         <v>0</v>
@@ -1075,7 +1075,7 @@
         <v>0</v>
       </c>
       <c r="F11" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G11" s="1">
         <v>0</v>
@@ -1089,7 +1089,7 @@
         <v>17</v>
       </c>
       <c r="B12" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C12" s="1">
         <v>0</v>
@@ -1101,7 +1101,7 @@
         <v>1</v>
       </c>
       <c r="F12" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G12" s="1">
         <v>0</v>
@@ -1115,7 +1115,7 @@
         <v>18</v>
       </c>
       <c r="B13" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C13" s="1">
         <v>0</v>
@@ -1127,7 +1127,7 @@
         <v>1</v>
       </c>
       <c r="F13" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -1141,7 +1141,7 @@
         <v>19</v>
       </c>
       <c r="B14" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1">
         <v>0</v>
@@ -1153,7 +1153,7 @@
         <v>1</v>
       </c>
       <c r="F14" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -1167,7 +1167,7 @@
         <v>20</v>
       </c>
       <c r="B15" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15" s="1">
         <v>0</v>
@@ -1179,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="F15" s="1">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -1193,7 +1193,7 @@
         <v>21</v>
       </c>
       <c r="B16" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C16" s="1">
         <v>0</v>
@@ -1205,7 +1205,7 @@
         <v>1</v>
       </c>
       <c r="F16" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G16" s="1">
         <v>0</v>
@@ -1219,7 +1219,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C17" s="1">
         <v>0</v>
@@ -1231,7 +1231,7 @@
         <v>0</v>
       </c>
       <c r="F17" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G17" s="1">
         <v>0</v>
@@ -1245,7 +1245,7 @@
         <v>23</v>
       </c>
       <c r="B18" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" s="1">
         <v>0</v>
@@ -1257,7 +1257,7 @@
         <v>0</v>
       </c>
       <c r="F18" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G18" s="1">
         <v>0</v>
@@ -1271,7 +1271,7 @@
         <v>24</v>
       </c>
       <c r="B19" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" s="1">
         <v>0</v>
@@ -1283,7 +1283,7 @@
         <v>0</v>
       </c>
       <c r="F19" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19" s="1">
         <v>0</v>
@@ -1297,7 +1297,7 @@
         <v>25</v>
       </c>
       <c r="B20" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C20" s="1">
         <v>0</v>
@@ -1309,7 +1309,7 @@
         <v>0</v>
       </c>
       <c r="F20" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G20" s="1">
         <v>0</v>
@@ -1323,7 +1323,7 @@
         <v>26</v>
       </c>
       <c r="B21" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C21" s="1">
         <v>0</v>
@@ -1335,7 +1335,7 @@
         <v>0</v>
       </c>
       <c r="F21" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G21" s="1">
         <v>0</v>
@@ -1354,7 +1354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C133"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A47" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>

</xml_diff>